<commit_message>
Fix: Replaced fixed number by formula in Diff Eq sheet
Added small fix in calculation of Differential Equations spreadsheet
</commit_message>
<xml_diff>
--- a/Differential Equations - RK-2 & Milne.xlsx
+++ b/Differential Equations - RK-2 & Milne.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4dbaf62a2830c877/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramiro Olivencia\WebstormProjects\matematica-superior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAC93463-D5FB-4B5E-9434-4FC7D4EC1407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8135FDA-9785-438A-AF7D-AA380E641553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="17400" windowWidth="2400" windowHeight="585" xr2:uid="{9698BD8A-E2CE-40F8-9E42-F32DA4461660}"/>
+    <workbookView xWindow="345" yWindow="1380" windowWidth="13770" windowHeight="14445" xr2:uid="{9698BD8A-E2CE-40F8-9E42-F32DA4461660}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -185,13 +185,13 @@
     <t>Order</t>
   </si>
   <si>
-    <t>Full Step Error</t>
-  </si>
-  <si>
-    <t>Half Steps Error</t>
-  </si>
-  <si>
-    <t>Improved Full Step</t>
+    <t>From half h Err</t>
+  </si>
+  <si>
+    <t>From full h Err</t>
+  </si>
+  <si>
+    <t>Improved step</t>
   </si>
 </sst>
 </file>
@@ -1097,6 +1097,24 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1106,40 +1124,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
@@ -1175,31 +1166,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1523,17 +1523,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378CBF73-4B3E-4E2C-95E3-10DA6DC71F97}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J32" sqref="J32:O32"/>
+      <selection pane="topRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="8" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="35.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
@@ -1544,50 +1544,50 @@
     <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="96"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
       <c r="I2" s="1"/>
-      <c r="K2" s="68" t="s">
+      <c r="K2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="70"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="76"/>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99"/>
-      <c r="K3" s="94" t="s">
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="79"/>
+      <c r="K3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="96"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="73"/>
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="100" t="s">
+      <c r="C4" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="102"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
       <c r="J4" s="5"/>
       <c r="K4" s="6" t="s">
         <v>5</v>
@@ -1605,14 +1605,14 @@
     </row>
     <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="85"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="82"/>
       <c r="I5" s="1"/>
       <c r="J5" s="5"/>
       <c r="K5" s="11">
@@ -1631,7 +1631,7 @@
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="83" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -1646,8 +1646,8 @@
       <c r="F6" s="16">
         <v>100</v>
       </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="89"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
       <c r="J6" s="5"/>
       <c r="K6" s="17">
         <v>1</v>
@@ -1665,7 +1665,7 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="87"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="20" t="s">
         <v>13</v>
       </c>
@@ -1724,8 +1724,9 @@
         <f t="array" ref="G8">B8*FXY(D8+B8,E8+F8)</f>
         <v>-13.465170536607044</v>
       </c>
-      <c r="H8" s="23">
-        <v>87.323923867514864</v>
+      <c r="H8" s="28">
+        <f>E8+(1/2)*(F8+G8)</f>
+        <v>87.326820672290538</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="21"/>
@@ -1759,27 +1760,27 @@
       </c>
       <c r="E9" s="27">
         <f>H8</f>
-        <v>87.323923867514864</v>
+        <v>87.326820672290538</v>
       </c>
       <c r="F9" s="27" cm="1">
         <f t="array" ref="F9">B9*FXY(D9,E9)</f>
-        <v>-13.586352909320354</v>
+        <v>-13.585907325389083</v>
       </c>
       <c r="G9" s="27" cm="1">
         <f t="array" ref="G9">B9*FXY(D9+B9,E9+F9)</f>
-        <v>-16.056181444152589</v>
+        <v>-16.055463417075686</v>
       </c>
       <c r="H9" s="28">
         <f>E9+(1/2)*(F9+G9)</f>
-        <v>72.502656690778394</v>
-      </c>
-      <c r="K9" s="94" t="s">
+        <v>72.506135301058151</v>
+      </c>
+      <c r="K9" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="95"/>
-      <c r="M9" s="95"/>
-      <c r="N9" s="95"/>
-      <c r="O9" s="96"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="73"/>
       <c r="P9" s="29"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1796,19 +1797,19 @@
       </c>
       <c r="E10" s="28">
         <f>H9</f>
-        <v>72.502656690778394</v>
+        <v>72.506135301058151</v>
       </c>
       <c r="F10" s="28" cm="1">
         <f t="array" ref="F10">B10*FXY(D10,E10)</f>
-        <v>-16.325940503733538</v>
+        <v>-16.325167893607453</v>
       </c>
       <c r="G10" s="28" cm="1">
         <f t="array" ref="G10">B10*FXY(D10+B10,E10+F10)</f>
-        <v>-20.987564169904125</v>
+        <v>-20.986003812234202</v>
       </c>
       <c r="H10" s="28">
         <f>E10+(1/2)*(F10+G10)</f>
-        <v>53.845904353959561</v>
+        <v>53.850549448137322</v>
       </c>
       <c r="K10" s="30"/>
       <c r="L10" s="31"/>
@@ -1835,19 +1836,19 @@
       </c>
       <c r="E11" s="28">
         <f>H10</f>
-        <v>53.845904353959561</v>
+        <v>53.850549448137322</v>
       </c>
       <c r="F11" s="28" cm="1">
         <f t="array" ref="F11">B11*FXY(D11,E11)</f>
-        <v>-21.879482417785436</v>
+        <v>-21.87762952374128</v>
       </c>
       <c r="G11" s="28" cm="1">
         <f t="array" ref="G11">B11*FXY(D11+B11,E11+F11)</f>
-        <v>-36.400674672043714</v>
+        <v>-36.393501174645522</v>
       </c>
       <c r="H11" s="28">
         <f>E11+(1/2)*(F11+G11)</f>
-        <v>24.705825809044988</v>
+        <v>24.714984098943923</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>10</v>
@@ -2230,14 +2231,14 @@
       <c r="P26" s="50"/>
     </row>
     <row r="27" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="94" t="s">
+      <c r="C27" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="96"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="73"/>
       <c r="J27" s="28"/>
       <c r="K27" s="17"/>
       <c r="L27" s="18"/>
@@ -2247,14 +2248,14 @@
       <c r="P27" s="50"/>
     </row>
     <row r="28" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="97" t="s">
+      <c r="C28" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="99"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="79"/>
       <c r="J28" s="23"/>
       <c r="K28" s="45"/>
       <c r="L28" s="46"/>
@@ -2264,27 +2265,27 @@
       <c r="P28" s="54"/>
     </row>
     <row r="29" spans="2:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="C29" s="100" t="s">
+      <c r="C29" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="101"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="102"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="70"/>
     </row>
     <row r="30" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="83" t="s">
+      <c r="C30" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="84"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="82"/>
     </row>
     <row r="31" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="86" t="s">
+      <c r="B31" s="83" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="15" t="s">
@@ -2299,11 +2300,11 @@
       <c r="F31" s="16">
         <v>2.33</v>
       </c>
-      <c r="G31" s="88"/>
-      <c r="H31" s="89"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="86"/>
     </row>
     <row r="32" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="87"/>
+      <c r="B32" s="84"/>
       <c r="C32" s="20" t="s">
         <v>13</v>
       </c>
@@ -2322,14 +2323,14 @@
       <c r="H32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="68" t="s">
+      <c r="J32" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="69"/>
-      <c r="O32" s="70"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="75"/>
+      <c r="O32" s="76"/>
       <c r="Q32">
         <v>2</v>
       </c>
@@ -2364,21 +2365,21 @@
         <f>E33+(1/2)*(F33+G33)</f>
         <v>91.957529050856465</v>
       </c>
-      <c r="J33" s="90">
+      <c r="J33" s="87">
         <f>Q32</f>
         <v>2</v>
       </c>
-      <c r="K33" s="91"/>
-      <c r="L33" s="92">
+      <c r="K33" s="88"/>
+      <c r="L33" s="89">
         <f>Q33</f>
         <v>3</v>
       </c>
-      <c r="M33" s="91"/>
-      <c r="N33" s="92">
+      <c r="M33" s="88"/>
+      <c r="N33" s="89">
         <f>Q34</f>
         <v>4</v>
       </c>
-      <c r="O33" s="93"/>
+      <c r="O33" s="90"/>
       <c r="Q33">
         <v>3</v>
       </c>
@@ -2414,21 +2415,21 @@
         <f>E34+(1/2)*(F34+G34)</f>
         <v>87.323923867514864</v>
       </c>
-      <c r="J34" s="77">
+      <c r="J34" s="97">
         <f>R32</f>
         <v>72.502656690778394</v>
       </c>
-      <c r="K34" s="78"/>
-      <c r="L34" s="79">
+      <c r="K34" s="98"/>
+      <c r="L34" s="99">
         <f>R33</f>
         <v>53.845904353959561</v>
       </c>
-      <c r="M34" s="78"/>
-      <c r="N34" s="79">
+      <c r="M34" s="98"/>
+      <c r="N34" s="99">
         <f>R34</f>
         <v>23.699792128613069</v>
       </c>
-      <c r="O34" s="80"/>
+      <c r="O34" s="100"/>
       <c r="Q34">
         <v>4</v>
       </c>
@@ -2464,16 +2465,16 @@
         <f>E35+(1/2)*(F35+G35)</f>
         <v>80.247742241134205</v>
       </c>
-      <c r="K35" s="81">
+      <c r="K35" s="101">
         <f>(L34-J34)/(L33-J33)</f>
         <v>-18.656752336818833</v>
       </c>
-      <c r="L35" s="82"/>
-      <c r="M35" s="81">
+      <c r="L35" s="102"/>
+      <c r="M35" s="101">
         <f>(N34-L34)/(N33-L33)</f>
         <v>-30.146112225346492</v>
       </c>
-      <c r="N35" s="82"/>
+      <c r="N35" s="102"/>
     </row>
     <row r="36" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="28"/>
@@ -2483,11 +2484,11 @@
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
-      <c r="L36" s="81">
+      <c r="L36" s="101">
         <f>(N33-J33)/(M35-K35)</f>
         <v>-0.1740741015517355</v>
       </c>
-      <c r="M36" s="82"/>
+      <c r="M36" s="102"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B37" s="28"/>
@@ -2515,21 +2516,21 @@
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
-      <c r="J39" s="68" t="s">
+      <c r="J39" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="K39" s="69"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="69"/>
-      <c r="N39" s="70"/>
-      <c r="O39" s="68" t="s">
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
+      <c r="M39" s="75"/>
+      <c r="N39" s="76"/>
+      <c r="O39" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="P39" s="70"/>
-      <c r="Q39" s="71">
+      <c r="P39" s="76"/>
+      <c r="Q39" s="91">
         <v>50</v>
       </c>
-      <c r="R39" s="72"/>
+      <c r="R39" s="92"/>
     </row>
     <row r="40" spans="2:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="28"/>
@@ -2539,18 +2540,18 @@
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
-      <c r="J40" s="71" t="str">
+      <c r="J40" s="91" t="str">
         <f>SUBSTITUTE(_xlfn.CONCAT("solve ",Q39," = ",J34, " + (", K35, ") * (t - ", J33, ") + (", L36,") * (t -",J33,") * (t - ", L33, ")"), ",", ".")</f>
         <v>solve 50 = 72.5026566907784 + (-18.6567523368188) * (t - 2) + (-0.174074101551735) * (t -2) * (t - 3)</v>
       </c>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="73"/>
-      <c r="N40" s="73"/>
-      <c r="O40" s="73"/>
-      <c r="P40" s="73"/>
-      <c r="Q40" s="73"/>
-      <c r="R40" s="72"/>
+      <c r="K40" s="93"/>
+      <c r="L40" s="93"/>
+      <c r="M40" s="93"/>
+      <c r="N40" s="93"/>
+      <c r="O40" s="93"/>
+      <c r="P40" s="93"/>
+      <c r="Q40" s="93"/>
+      <c r="R40" s="92"/>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B41" s="28"/>
@@ -2635,15 +2636,15 @@
     </row>
     <row r="50" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="74" t="s">
+      <c r="B51" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="75"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="76"/>
+      <c r="C51" s="95"/>
+      <c r="D51" s="95"/>
+      <c r="E51" s="95"/>
+      <c r="F51" s="95"/>
+      <c r="G51" s="95"/>
+      <c r="H51" s="96"/>
     </row>
     <row r="52" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" s="57"/>
@@ -2698,54 +2699,32 @@
     </row>
     <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="66" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C55" s="67">
         <f>((2^H53)/(1-2^H53))*(G53-F53)</f>
         <v>-3.862406367564593E-3</v>
       </c>
       <c r="D55" s="66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E55" s="67">
         <v>-4.2444026017193336E-3</v>
       </c>
-      <c r="F55" s="68" t="s">
+      <c r="F55" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="G55" s="70"/>
+      <c r="G55" s="76"/>
       <c r="H55" s="33">
         <f>G53+C55</f>
         <v>87.322958265922978</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F57">
-        <f>(F53-G53)/(1-0.65^3-0.35^3)</f>
-        <v>-4.2444026017193336E-3</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="K9:O9"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="J40:R40"/>
+    <mergeCell ref="B51:H51"/>
     <mergeCell ref="F55:G55"/>
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="L34:M34"/>
@@ -2755,9 +2734,25 @@
     <mergeCell ref="L36:M36"/>
     <mergeCell ref="J39:N39"/>
     <mergeCell ref="O39:P39"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="J40:R40"/>
-    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K9:O9"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J46" r:id="rId1" xr:uid="{FC08842B-FEBC-4DA5-AE26-3E7B3A379D0A}"/>

</xml_diff>